<commit_message>
Updating writing excel code
</commit_message>
<xml_diff>
--- a/src/main/java/com/mystore/qa/testdata/MyStoreData.xlsx
+++ b/src/main/java/com/mystore/qa/testdata/MyStoreData.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Backup" sheetId="1" r:id="rId1"/>
-    <sheet name="Search Items" sheetId="2" r:id="rId2"/>
+    <sheet name="Search Items" sheetId="2" r:id="rId1"/>
+    <sheet name="TestSheet" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Items</t>
   </si>
@@ -38,6 +38,33 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Richa</t>
+  </si>
+  <si>
+    <t>Chandigarh</t>
+  </si>
+  <si>
+    <t>Shikha</t>
+  </si>
+  <si>
+    <t>Gurgaon</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>PASSED</t>
   </si>
 </sst>
 </file>
@@ -412,40 +439,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>7</v>
       </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -455,40 +492,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
         <v>7</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>